<commit_message>
update system test report for Rhythm hospital.
</commit_message>
<xml_diff>
--- a/Library/excelResultSystemTest_RTMV2.1.8F.xlsx
+++ b/Library/excelResultSystemTest_RTMV2.1.8F.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24228" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="26100" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -175,24 +175,15 @@
     <t>TC021</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC001CashCollectionSummaryReport.py</t>
-  </si>
-  <si>
     <t>TC022</t>
   </si>
   <si>
     <t>script enhancement</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC002UserCollectionReport.py</t>
-  </si>
-  <si>
     <t>TC023</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC006Opening&amp;EndingStockSummaryReport.py</t>
-  </si>
-  <si>
     <t>Failed</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>TC037</t>
   </si>
   <si>
-    <t>Remove not available</t>
-  </si>
-  <si>
     <t>Reports\TC004PatientCensusReport.py</t>
   </si>
   <si>
@@ -440,6 +428,18 @@
   </si>
   <si>
     <t>EMR-4917</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC001CashCollectionSummaryReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Sales\TC002UserCollectionReport.py</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\Stock\TC006Opening&amp;EndingStockSummaryReport.py</t>
+  </si>
+  <si>
+    <t>Report not available</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1203,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="ManualStatus">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="ManualStatus">
   <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1610,18 +1610,18 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
@@ -1633,18 +1633,18 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" t="s">
         <v>131</v>
       </c>
-      <c r="G4" t="s">
-        <v>135</v>
-      </c>
       <c r="H4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" s="12">
         <v>6</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" s="12">
         <v>6</v>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2130,7 +2130,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2202,12 +2202,12 @@
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>9</v>
@@ -2219,17 +2219,17 @@
         <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>9</v>
@@ -2241,19 +2241,19 @@
         <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>9</v>
@@ -2265,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>13</v>
@@ -2275,10 +2275,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>10</v>
@@ -2287,19 +2287,19 @@
         <v>2</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>13</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>9</v>
@@ -2331,7 +2331,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>13</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>13</v>
@@ -2353,19 +2353,19 @@
         <v>2</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>13</v>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>13</v>
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>13</v>
@@ -2417,19 +2417,19 @@
         <v>2</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>13</v>
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>44</v>
@@ -2461,22 +2461,22 @@
         <v>2</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>44</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="9" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>10</v>
@@ -2485,19 +2485,19 @@
         <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>13</v>
@@ -2509,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>13</v>
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>13</v>
@@ -2549,7 +2549,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>13</v>
@@ -2569,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>13</v>
@@ -2589,19 +2589,19 @@
         <v>2</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>13</v>
@@ -2613,19 +2613,19 @@
         <v>2</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>13</v>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>13</v>
@@ -2657,19 +2657,19 @@
         <v>2</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>13</v>
@@ -2681,19 +2681,19 @@
         <v>2</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>13</v>
@@ -2705,7 +2705,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>13</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>13</v>
@@ -2727,22 +2727,22 @@
         <v>2</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>10</v>
@@ -2751,21 +2751,21 @@
         <v>2</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>13</v>
@@ -2777,7 +2777,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>13</v>
@@ -2786,10 +2786,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>10</v>
@@ -2798,22 +2798,22 @@
         <v>2</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>10</v>
@@ -2822,24 +2822,24 @@
         <v>5</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>10</v>
@@ -2848,24 +2848,24 @@
         <v>5</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>10</v>
@@ -2874,16 +2874,16 @@
         <v>5</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>